<commit_message>
Calc with Rg parameter
</commit_message>
<xml_diff>
--- a/devices/Cree_C3M0015065K_SiC_650V.xlsx
+++ b/devices/Cree_C3M0015065K_SiC_650V.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Forward" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Ron_vs_Tj</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -107,6 +107,10 @@
   </si>
   <si>
     <t>Zthch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eoff_vs_Rg</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -469,24 +473,24 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.875" customWidth="1"/>
-    <col min="2" max="2" width="14.75" customWidth="1"/>
-    <col min="3" max="3" width="10.875" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.375" customWidth="1"/>
-    <col min="8" max="8" width="11.125" customWidth="1"/>
-    <col min="10" max="10" width="11.125" customWidth="1"/>
-    <col min="11" max="11" width="9.75" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" customWidth="1"/>
+    <col min="11" max="11" width="9.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -502,7 +506,7 @@
       <c r="H1" s="3"/>
       <c r="K1" s="3"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>-37.945669000000002</v>
       </c>
@@ -520,7 +524,7 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>-32.338952999999997</v>
       </c>
@@ -538,7 +542,7 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>-27.043721999999999</v>
       </c>
@@ -556,7 +560,7 @@
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>-21.74849</v>
       </c>
@@ -574,7 +578,7 @@
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>-15.726462</v>
       </c>
@@ -592,7 +596,7 @@
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>-9.3929495000000003</v>
       </c>
@@ -610,7 +614,7 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>-3.3709213</v>
       </c>
@@ -628,7 +632,7 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>3.4337061000000002</v>
       </c>
@@ -646,7 +650,7 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9.3652902999999998</v>
       </c>
@@ -664,7 +668,7 @@
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>15.570639999999999</v>
       </c>
@@ -682,7 +686,7 @@
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>21.867245</v>
       </c>
@@ -700,7 +704,7 @@
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>27.798829000000001</v>
       </c>
@@ -718,7 +722,7 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>33.000371999999999</v>
       </c>
@@ -736,7 +740,7 @@
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>39.023211000000003</v>
       </c>
@@ -754,7 +758,7 @@
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>45.411071</v>
       </c>
@@ -772,7 +776,7 @@
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>53.203353</v>
       </c>
@@ -790,7 +794,7 @@
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>61.671146</v>
       </c>
@@ -808,7 +812,7 @@
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>70.676576999999995</v>
       </c>
@@ -820,7 +824,7 @@
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>78.875551000000002</v>
       </c>
@@ -832,7 +836,7 @@
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>86.402478000000002</v>
       </c>
@@ -842,7 +846,7 @@
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>93.257357999999996</v>
       </c>
@@ -850,7 +854,7 @@
         <v>1.0678285999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>100.91869</v>
       </c>
@@ -858,7 +862,7 @@
         <v>1.086141</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>108.31121</v>
       </c>
@@ -866,7 +870,7 @@
         <v>1.1026222000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>115.70372999999999</v>
       </c>
@@ -875,7 +879,7 @@
       </c>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>123.26891999999999</v>
       </c>
@@ -884,7 +888,7 @@
       </c>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>131.19907000000001</v>
       </c>
@@ -893,7 +897,7 @@
       </c>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>137.51632000000001</v>
       </c>
@@ -902,7 +906,7 @@
       </c>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>143.96797000000001</v>
       </c>
@@ -911,7 +915,7 @@
       </c>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>149.74757</v>
       </c>
@@ -921,7 +925,7 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>155.66158999999999</v>
       </c>
@@ -929,7 +933,7 @@
         <v>1.2354761000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>161.71001000000001</v>
       </c>
@@ -937,7 +941,7 @@
         <v>1.2592823</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>168.16166000000001</v>
       </c>
@@ -945,7 +949,7 @@
         <v>1.279426</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>174.08756</v>
       </c>
@@ -965,22 +969,22 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.75" customWidth="1"/>
-    <col min="2" max="3" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" customWidth="1"/>
+    <col min="2" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="6" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.25" customWidth="1"/>
-    <col min="10" max="10" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.25" customWidth="1"/>
+    <col min="5" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.21875" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1001,7 +1005,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>2.7609935000000001</v>
       </c>
@@ -1023,7 +1027,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>8.3766473999999995</v>
       </c>
@@ -1045,7 +1049,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>16.800128000000001</v>
       </c>
@@ -1067,7 +1071,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>26.908304999999999</v>
       </c>
@@ -1089,7 +1093,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>37.858829999999998</v>
       </c>
@@ -1111,7 +1115,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>49.090138000000003</v>
       </c>
@@ -1133,7 +1137,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>58.355967</v>
       </c>
@@ -1155,7 +1159,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>70.148840000000007</v>
       </c>
@@ -1177,7 +1181,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>79.695452000000003</v>
       </c>
@@ -1199,7 +1203,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>88.680498</v>
       </c>
@@ -1217,7 +1221,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>99.786106000000004</v>
       </c>
@@ -1231,7 +1235,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>111.03139</v>
       </c>
@@ -1245,7 +1249,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="D14" s="2"/>
@@ -1255,7 +1259,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="D15" s="2"/>
@@ -1265,7 +1269,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="D16" s="2"/>
@@ -1275,7 +1279,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="D17" s="2"/>
@@ -1285,7 +1289,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="D18" s="2"/>
@@ -1295,7 +1299,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="D19" s="2"/>
@@ -1305,7 +1309,7 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="D20" s="2"/>
@@ -1313,7 +1317,7 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="1"/>
@@ -1322,7 +1326,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="1"/>
@@ -1331,7 +1335,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="1"/>
@@ -1340,14 +1344,14 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="E25" s="1"/>
@@ -1355,7 +1359,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="E26" s="1"/>
@@ -1363,7 +1367,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="E27" s="1"/>
@@ -1371,7 +1375,7 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="E28" s="1"/>
@@ -1393,27 +1397,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10:N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="12.75" customWidth="1"/>
-    <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.125" customWidth="1"/>
-    <col min="5" max="5" width="15.25" customWidth="1"/>
-    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.25" customWidth="1"/>
-    <col min="10" max="10" width="11.125" customWidth="1"/>
-    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="15.21875" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.21875" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" customWidth="1"/>
+    <col min="11" max="11" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1439,7 +1443,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>13.059264000000001</v>
       </c>
@@ -1462,8 +1466,14 @@
         <v>3.5387020999999997E-4</v>
       </c>
       <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J2" s="2">
+        <v>2.5217556000000001</v>
+      </c>
+      <c r="K2" s="2">
+        <v>2.3764815E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>17.731895999999999</v>
       </c>
@@ -1486,8 +1496,14 @@
         <v>3.5514197000000003E-4</v>
       </c>
       <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J3" s="2">
+        <v>3.7981438000000001</v>
+      </c>
+      <c r="K3" s="2">
+        <v>2.8704985000000001E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>22.771008999999999</v>
       </c>
@@ -1510,8 +1526,14 @@
         <v>3.5514197000000003E-4</v>
       </c>
       <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J4" s="2">
+        <v>4.8675500999999999</v>
+      </c>
+      <c r="K4" s="2">
+        <v>3.3233474000000002E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>26.710678999999999</v>
       </c>
@@ -1534,8 +1556,14 @@
         <v>3.5768549E-4</v>
       </c>
       <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J5" s="2">
+        <v>6.2301807</v>
+      </c>
+      <c r="K5" s="2">
+        <v>3.8379484999999998E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>30.833589</v>
       </c>
@@ -1558,8 +1586,14 @@
         <v>3.6022901000000001E-4</v>
       </c>
       <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J6" s="2">
+        <v>7.4375749000000004</v>
+      </c>
+      <c r="K6" s="2">
+        <v>4.3731336000000002E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>34.681638999999997</v>
       </c>
@@ -1582,8 +1616,14 @@
         <v>3.6404428999999998E-4</v>
       </c>
       <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J7" s="2">
+        <v>8.6277206999999994</v>
+      </c>
+      <c r="K7" s="2">
+        <v>4.8671506000000001E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>38.621310000000001</v>
       </c>
@@ -1606,8 +1646,14 @@
         <v>3.6658780999999999E-4</v>
       </c>
       <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J8" s="2">
+        <v>9.8523633999999998</v>
+      </c>
+      <c r="K8" s="2">
+        <v>5.3611676999999996E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>42.377738999999998</v>
       </c>
@@ -1630,8 +1676,14 @@
         <v>3.7040309000000002E-4</v>
       </c>
       <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J9" s="2">
+        <v>10.990764</v>
+      </c>
+      <c r="K9" s="2">
+        <v>5.8140166000000002E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>46.409030000000001</v>
       </c>
@@ -1654,8 +1706,14 @@
         <v>3.7549013000000005E-4</v>
       </c>
       <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J10" s="2">
+        <v>12.129163999999999</v>
+      </c>
+      <c r="K10" s="2">
+        <v>6.2874496000000005E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>49.982219000000001</v>
       </c>
@@ -1678,8 +1736,14 @@
         <v>3.8057717000000002E-4</v>
       </c>
       <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J11" s="2">
+        <v>13.491795</v>
+      </c>
+      <c r="K11" s="2">
+        <v>6.8226346999999998E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>55.763033</v>
       </c>
@@ -1702,8 +1766,14 @@
         <v>3.8590496000000002E-4</v>
       </c>
       <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J12" s="2">
+        <v>14.681940000000001</v>
+      </c>
+      <c r="K12" s="2">
+        <v>7.2960677000000001E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>60.942630000000001</v>
       </c>
@@ -1726,8 +1796,14 @@
         <v>3.9281249000000003E-4</v>
       </c>
       <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J13" s="2">
+        <v>15.837588999999999</v>
+      </c>
+      <c r="K13" s="2">
+        <v>7.8106688000000003E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>65.535858000000005</v>
       </c>
@@ -1750,8 +1826,14 @@
         <v>4.0144690000000005E-4</v>
       </c>
       <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J14" s="2">
+        <v>16.993238000000002</v>
+      </c>
+      <c r="K14" s="2">
+        <v>8.2223495999999999E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>70.422270999999995</v>
       </c>
@@ -1767,8 +1849,14 @@
         <v>0.96772828186022253</v>
       </c>
       <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J15" s="2">
+        <v>17.936558999999999</v>
+      </c>
+      <c r="K15" s="2">
+        <v>8.6160347999999999E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>74.820042000000001</v>
       </c>
@@ -1784,8 +1872,14 @@
         <v>0.99897608517236991</v>
       </c>
       <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="J16" s="2">
+        <v>18.846146999999998</v>
+      </c>
+      <c r="K16" s="2">
+        <v>9.0061315000000003E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>79.510998000000001</v>
       </c>
@@ -1793,8 +1887,14 @@
         <v>5.6131437000000008E-4</v>
       </c>
       <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="J17" s="2">
+        <v>19.78416</v>
+      </c>
+      <c r="K17" s="2">
+        <v>9.3792675999999995E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>84.104225999999997</v>
       </c>
@@ -1803,7 +1903,7 @@
       </c>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>88.404268999999999</v>
       </c>
@@ -1812,7 +1912,7 @@
       </c>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>92.606583999999998</v>
       </c>
@@ -1821,7 +1921,7 @@
       </c>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>96.515714000000003</v>
       </c>
@@ -1830,12 +1930,12 @@
       </c>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1852,24 +1952,24 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G9"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5" customWidth="1"/>
-    <col min="5" max="5" width="15.25" customWidth="1"/>
-    <col min="6" max="7" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5" customWidth="1"/>
-    <col min="9" max="9" width="11.25" customWidth="1"/>
-    <col min="10" max="10" width="12.25" customWidth="1"/>
-    <col min="11" max="11" width="12.375" customWidth="1"/>
-    <col min="12" max="12" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.375" customWidth="1"/>
+    <col min="1" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.21875" customWidth="1"/>
+    <col min="6" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" customWidth="1"/>
+    <col min="9" max="9" width="11.21875" customWidth="1"/>
+    <col min="10" max="10" width="12.21875" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" customWidth="1"/>
+    <col min="12" max="12" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -1888,8 +1988,14 @@
       <c r="H1" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>13.496788</v>
       </c>
@@ -1912,8 +2018,14 @@
         <v>2.3855779999999997E-4</v>
       </c>
       <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J2" s="2">
+        <v>2.5543741999999998</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1.5241235E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>17.353797</v>
       </c>
@@ -1936,8 +2048,14 @@
         <v>2.4140881999999998E-4</v>
       </c>
       <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J3" s="2">
+        <v>3.8307623999999998</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1.9975565000000001E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>21.732022000000001</v>
       </c>
@@ -1960,8 +2078,14 @@
         <v>2.4252709E-4</v>
       </c>
       <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J4" s="2">
+        <v>4.9519142</v>
+      </c>
+      <c r="K4" s="2">
+        <v>2.3886533000000001E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>25.797518</v>
       </c>
@@ -1984,8 +2108,14 @@
         <v>2.4519673E-4</v>
       </c>
       <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J5" s="2">
+        <v>6.2283023000000002</v>
+      </c>
+      <c r="K5" s="2">
+        <v>2.8826703000000003E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>29.550281999999999</v>
       </c>
@@ -2008,8 +2138,14 @@
         <v>2.4786341999999997E-4</v>
       </c>
       <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J6" s="2">
+        <v>7.4356966</v>
+      </c>
+      <c r="K6" s="2">
+        <v>3.2943510999999999E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>33.824264999999997</v>
       </c>
@@ -2032,8 +2168,14 @@
         <v>2.5090087000000002E-4</v>
       </c>
       <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J7" s="2">
+        <v>8.8845696000000007</v>
+      </c>
+      <c r="K7" s="2">
+        <v>3.8089522000000001E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>38.723708000000002</v>
       </c>
@@ -2056,8 +2198,14 @@
         <v>2.5364828E-4</v>
       </c>
       <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J8" s="2">
+        <v>10.126461000000001</v>
+      </c>
+      <c r="K8" s="2">
+        <v>4.3029692E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>42.476472999999999</v>
       </c>
@@ -2080,8 +2228,14 @@
         <v>2.5440764E-4</v>
       </c>
       <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J9" s="2">
+        <v>11.50634</v>
+      </c>
+      <c r="K9" s="2">
+        <v>4.7969863E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>46.541967999999997</v>
       </c>
@@ -2097,11 +2251,19 @@
         <v>0.81629104413588016</v>
       </c>
       <c r="F10" s="2"/>
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J10" s="2">
+        <v>13.213939999999999</v>
+      </c>
+      <c r="K10" s="2">
+        <v>5.4145075999999996E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>50.398975999999998</v>
       </c>
@@ -2119,9 +2281,14 @@
       <c r="F11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J11" s="2">
+        <v>14.69731</v>
+      </c>
+      <c r="K11" s="2">
+        <v>5.9496926999999999E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>54.360227999999999</v>
       </c>
@@ -2139,9 +2306,14 @@
       <c r="F12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J12" s="2">
+        <v>16.163432</v>
+      </c>
+      <c r="K12" s="2">
+        <v>6.4642937000000005E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>57.904505999999998</v>
       </c>
@@ -2159,9 +2331,14 @@
       <c r="F13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J13" s="2">
+        <v>17.577808000000001</v>
+      </c>
+      <c r="K13" s="2">
+        <v>6.9788947999999996E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>62.386975</v>
       </c>
@@ -2179,9 +2356,14 @@
       <c r="F14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J14" s="2">
+        <v>18.823346000000001</v>
+      </c>
+      <c r="K14" s="2">
+        <v>7.4663933999999995E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>66.660956999999996</v>
       </c>
@@ -2199,9 +2381,14 @@
       <c r="F15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J15" s="2">
+        <v>19.783614</v>
+      </c>
+      <c r="K15" s="2">
+        <v>7.8157735999999996E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>70.413722000000007</v>
       </c>
@@ -2214,7 +2401,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>74.270730999999998</v>
       </c>
@@ -2223,7 +2410,7 @@
       </c>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>78.386583000000002</v>
       </c>
@@ -2232,7 +2419,7 @@
       </c>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>82.236714000000006</v>
       </c>
@@ -2241,7 +2428,7 @@
       </c>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>85.860365000000002</v>
       </c>
@@ -2250,7 +2437,7 @@
       </c>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>89.484016999999994</v>
       </c>
@@ -2259,7 +2446,7 @@
       </c>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>92.277248999999998</v>
       </c>
@@ -2268,7 +2455,7 @@
       </c>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>95.372451999999996</v>
       </c>
@@ -2277,7 +2464,7 @@
       </c>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>98.014697999999996</v>
       </c>
@@ -2297,13 +2484,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -2314,7 +2501,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.35</v>
       </c>
@@ -2328,7 +2515,7 @@
         <v>2.8960000000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -2339,7 +2526,7 @@
         <v>3.5379999999999999E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D4" s="4">
         <v>2.531E-6</v>
       </c>
@@ -2347,7 +2534,7 @@
         <v>4.4819999999999999E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D5" s="4">
         <v>3.9020000000000001E-6</v>
       </c>
@@ -2355,7 +2542,7 @@
         <v>5.5259999999999997E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D6" s="4">
         <v>5.7189999999999998E-6</v>
       </c>
@@ -2363,7 +2550,7 @@
         <v>6.5690000000000002E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D7" s="4">
         <v>8.3809999999999999E-6</v>
       </c>
@@ -2371,7 +2558,7 @@
         <v>7.953E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D8" s="4">
         <v>1.0020000000000001E-5</v>
       </c>
@@ -2379,7 +2566,7 @@
         <v>8.7899999999999992E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D9" s="4">
         <v>1.525E-5</v>
       </c>
@@ -2387,7 +2574,7 @@
         <v>1.0840000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D10" s="4">
         <v>2.264E-5</v>
       </c>
@@ -2395,7 +2582,7 @@
         <v>1.324E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D11" s="4">
         <v>3.1529999999999998E-5</v>
       </c>
@@ -2403,7 +2590,7 @@
         <v>1.532E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D12" s="4">
         <v>4.3900000000000003E-5</v>
       </c>
@@ -2411,7 +2598,7 @@
         <v>1.821E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D13" s="4">
         <v>6.5160000000000006E-5</v>
       </c>
@@ -2419,7 +2606,7 @@
         <v>2.2040000000000001E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D14" s="4">
         <v>8.7349999999999995E-5</v>
       </c>
@@ -2427,7 +2614,7 @@
         <v>2.5499999999999998E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D15" s="4">
         <v>1.2579999999999999E-4</v>
       </c>
@@ -2435,7 +2622,7 @@
         <v>3.1289999999999998E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D16" s="4">
         <v>1.76E-4</v>
       </c>
@@ -2443,7 +2630,7 @@
         <v>3.635E-2</v>
       </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D17" s="4">
         <v>2.4620000000000002E-4</v>
       </c>
@@ -2451,7 +2638,7 @@
         <v>4.3189999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D18" s="4">
         <v>3.5179999999999999E-4</v>
       </c>
@@ -2459,7 +2646,7 @@
         <v>5.1319999999999998E-2</v>
       </c>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D19" s="4">
         <v>4.9220000000000004E-4</v>
       </c>
@@ -2467,7 +2654,7 @@
         <v>6.191E-2</v>
       </c>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D20" s="4">
         <v>6.96E-4</v>
       </c>
@@ -2475,7 +2662,7 @@
         <v>7.4109999999999995E-2</v>
       </c>
     </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D21" s="4">
         <v>9.9449999999999994E-4</v>
       </c>
@@ -2483,7 +2670,7 @@
         <v>8.9399999999999993E-2</v>
       </c>
     </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D22" s="4">
         <v>1.513E-3</v>
       </c>
@@ -2491,7 +2678,7 @@
         <v>0.1125</v>
       </c>
     </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D23" s="4">
         <v>2.653E-3</v>
       </c>
@@ -2499,7 +2686,7 @@
         <v>0.14410000000000001</v>
       </c>
     </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D24" s="4">
         <v>3.8869999999999998E-3</v>
       </c>
@@ -2507,7 +2694,7 @@
         <v>0.1651</v>
       </c>
     </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D25" s="4">
         <v>5.4310000000000001E-3</v>
       </c>
@@ -2515,7 +2702,7 @@
         <v>0.18609999999999999</v>
       </c>
     </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D26" s="4">
         <v>7.7710000000000001E-3</v>
       </c>
@@ -2523,7 +2710,7 @@
         <v>0.2079</v>
       </c>
     </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D27" s="4">
         <v>1.125E-2</v>
       </c>
@@ -2531,7 +2718,7 @@
         <v>0.23230000000000001</v>
       </c>
     </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D28" s="4">
         <v>1.5720000000000001E-2</v>
       </c>
@@ -2539,7 +2726,7 @@
         <v>0.25519999999999998</v>
       </c>
     </row>
-    <row r="29" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D29" s="4">
         <v>2.223E-2</v>
       </c>
@@ -2547,7 +2734,7 @@
         <v>0.28029999999999999</v>
       </c>
     </row>
-    <row r="30" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D30" s="4">
         <v>3.2190000000000003E-2</v>
       </c>
@@ -2555,7 +2742,7 @@
         <v>0.30520000000000003</v>
       </c>
     </row>
-    <row r="31" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="31" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D31" s="4">
         <v>5.1670000000000001E-2</v>
       </c>
@@ -2563,7 +2750,7 @@
         <v>0.33110000000000001</v>
       </c>
     </row>
-    <row r="32" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D32" s="4">
         <v>8.2059999999999994E-2</v>
       </c>
@@ -2571,7 +2758,7 @@
         <v>0.34050000000000002</v>
       </c>
     </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D33" s="4">
         <v>0.1303</v>
       </c>
@@ -2579,7 +2766,7 @@
         <v>0.3478</v>
       </c>
     </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D34" s="4">
         <v>0.2195</v>
       </c>
@@ -2587,7 +2774,7 @@
         <v>0.3503</v>
       </c>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D35" s="4">
         <v>0.31669999999999998</v>
       </c>
@@ -2595,7 +2782,7 @@
         <v>0.34949999999999998</v>
       </c>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D36" s="4">
         <v>0.44</v>
       </c>
@@ -2603,7 +2790,7 @@
         <v>0.34949999999999998</v>
       </c>
     </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D37" s="4">
         <v>0.59550000000000003</v>
       </c>
@@ -2611,7 +2798,7 @@
         <v>0.34949999999999998</v>
       </c>
     </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D38" s="4">
         <v>0.75870000000000004</v>
       </c>
@@ -2619,7 +2806,7 @@
         <v>0.34949999999999998</v>
       </c>
     </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D39" s="4">
         <v>0.91769999999999996</v>
       </c>

</xml_diff>